<commit_message>
Complete 152 Maximum Product Subarray
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Code\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A6B929-0400-4309-BD94-97C7A5FFEFDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9612B6B-1296-497B-BD3F-6BD6C90189B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4F5271F9-EB41-4AA5-937E-D997D947604F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{4F5271F9-EB41-4AA5-937E-D997D947604F}"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
   <si>
     <t>#</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>Traverse tree using a traverse(node) function. Check if node is NULL; traverse left then check if k == count; check current node; traverse right.</t>
+  </si>
+  <si>
+    <t>Maximum Product Subarray</t>
   </si>
 </sst>
 </file>
@@ -235,18 +238,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -261,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -282,7 +279,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1126,10 +1122,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1082AEA-234F-4AF9-BE46-F9132E309B8F}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1181,7 +1177,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="120" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="A3">
         <v>11</v>
       </c>
       <c r="B3" t="s">
@@ -1213,7 +1209,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="150" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+      <c r="A4">
         <v>23</v>
       </c>
       <c r="B4" t="s">
@@ -1245,7 +1241,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="195" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="A5">
         <v>53</v>
       </c>
       <c r="B5" t="s">
@@ -1277,7 +1273,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="180" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6">
         <v>82</v>
       </c>
       <c r="B6" t="s">
@@ -1309,7 +1305,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="150" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="A7">
         <v>98</v>
       </c>
       <c r="B7" t="s">
@@ -1341,7 +1337,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="150" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="A8">
         <v>147</v>
       </c>
       <c r="B8" t="s">
@@ -1369,7 +1365,7 @@
       <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" ht="180" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="A9">
         <v>148</v>
       </c>
       <c r="B9" t="s">
@@ -1398,15 +1394,15 @@
       </c>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:10" ht="195" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
-        <v>215</v>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>152</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="C10" s="4">
-        <v>45039</v>
+        <v>45091</v>
       </c>
       <c r="D10" t="s">
         <v>22</v>
@@ -1414,24 +1410,18 @@
       <c r="E10" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>56</v>
-      </c>
+      <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>58</v>
-      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
-        <v>230</v>
+    <row r="11" spans="1:10" ht="195" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>215</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="4">
         <v>45039</v>
@@ -1443,23 +1433,23 @@
         <v>23</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
-        <v>2181</v>
+    <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>230</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="4">
         <v>45039</v>
@@ -1470,11 +1460,39 @@
       <c r="E12" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="6"/>
+      <c r="F12" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
+      <c r="H12" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2181</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="4">
+        <v>45039</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>